<commit_message>
backup prima della morte
</commit_message>
<xml_diff>
--- a/NIST controls baselines_tabella semplificata.xlsx
+++ b/NIST controls baselines_tabella semplificata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\greenhouseSSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B157C5-0767-4452-8FFD-1C160F8FEC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506D86B2-9DE7-4858-99DD-F6A2ED4EEA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EAF0359E-8923-4E23-A0F3-A24CEB3062AA}"/>
   </bookViews>
@@ -5206,10 +5206,10 @@
     <t>Non ancora specificato. Si fa uso di java e javascript.</t>
   </si>
   <si>
-    <t>Le chiavi RSA sono state generate tramite OpenSSL, distribuite fisicamente tra le varie componenti dell'infrastruttura (mount di volumi e segreti di docker), ove possibile (Spring, Keycloak) sono state messe in keystore protetti da password con entry a loro volte protette da password. Ove non possibile, (MariaDB, Mosquitto, PostgreSQL) per i programmi che richiedevano file di chiavi non crittati e non in keystore, sono stati limitati gli accessi ai soli possessori delle chiavi e in sola lettura, e sono stati configurati appositamente i permessi anche nelle relative cartelle che li contengono. Le password per accedere ai keystore sono contenute in file di configurazione che vengono inclusi nell'eseguibile. Le connessioni SSL generano chiavi simmetriche di sessione ogni volta. Le password per i keystore e truststore nel caso del webserver sono contenute dentro il codice, che pertanto deve essere cifrato per evitare reverse engineering. Non sono state messe password nei file di configurazione di hibernate dato che quando viene impacchettato nel jar sono in chiaro.</t>
-  </si>
-  <si>
     <t>Creazione delle risorse su keycloak, scopes associati, permission sugli scopes e policy abac e rbac necessarie. Abilitazione dell'enforcement delle policy e protezione dei path ad accesso ristretto del server tramite lo springboot adapter per keycloak. Configurazione dei database per permettere l'accesso solo a chi ha ID,password e certificati necessari firmati dalla CA root e, nel caso di MariaDB, che rispettino anche i campi richiesti dal DB. Configurazione dei permessi dei file delle chiavi, dei certificati, dei file di configurazione delle varie parti dell'infrastruttura al fine di dare accesso solo al proprietario del file o al gruppo ove necessario.  Crittazione con password base encrryption del file config.xml per il web server java, garantisce accesso anche in caso di password errata, ma il file avrà un formato errato e il server si arresterà.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le chiavi RSA sono state generate tramite OpenSSL, distribuite fisicamente tra le varie componenti dell'infrastruttura (mount di volumi e segreti di docker), ove possibile (Spring, Keycloak) sono state messe in keystore protetti da password con entry a loro volte protette da password. Ove non possibile, (MariaDB, Mosquitto, PostgreSQL) per i programmi che richiedevano file di chiavi non crittati e non in keystore, sono stati limitati gli accessi ai soli possessori delle chiavi e in sola lettura, e sono stati configurati appositamente i permessi anche nelle relative cartelle che li contengono. Le password per accedere ai keystore sono immesse da tastiera all'avvio del web server, è compito del responsabile software salvarle su un mezzo diverso. Le connessioni SSL generano chiavi simmetriche di sessione ogni volta. Le password per i keystore e truststore nel caso del webserver sono contenute dentro il codice, che pertanto deve essere cifrato per evitare reverse engineering. Non sono state messe password nei file di configurazione di hibernate dato che quando viene impacchettato nel jar sono in chiaro, bensì la password viene inserita nel codice java, è richiesta pertanto una tencica di obscuring per evitare la decompilazione. </t>
   </si>
 </sst>
 </file>
@@ -5715,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752914C7-115F-4905-A8A7-15F56CC9E2E7}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,7 +5815,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -8617,7 +8617,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>324</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>326</v>
       </c>
       <c r="G147" s="16" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rimozione della password dal codice java
</commit_message>
<xml_diff>
--- a/NIST controls baselines_tabella semplificata.xlsx
+++ b/NIST controls baselines_tabella semplificata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\greenhouseSSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC64BF-51F1-4F73-BBDE-9FE4842AD9F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE4146-95D2-4B99-8E6F-3EE175C5E617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EAF0359E-8923-4E23-A0F3-A24CEB3062AA}"/>
   </bookViews>
@@ -4779,9 +4779,6 @@
     <t>Non utilizzato</t>
   </si>
   <si>
-    <t>lol</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -5052,13 +5049,16 @@
     <t xml:space="preserve"> L'identificazione a livello dei database non è a granularità personale ma è regolata da ID legato all'applicazione,password e  inoltre si richiede un particolare IP. Inoltre le connessioni tra il server springboot e il database MariaDB, tra il server keycloak e il database Postgresql sono su canali ssl in mutua autenticazioni, in cui si verificano che i contenuti dei certificati siano quelli attesi. I firewall sono basati principalmente su IP filtering. La connessione al broker Mosquitto è regolata anche da username e password, oltre a una connessione ssl mutuamente autenticata.</t>
   </si>
   <si>
-    <t>Le chiavi RSA sono state generate tramite OpenSSL, distribuite fisicamente tra le varie componenti dell'infrastruttura (mount di volumi e segreti di docker), ove possibile (Spring, Keycloak) sono state messe in keystore protetti da password con entry a loro volte protette da password. Ove non possibile, (MariaDB, Mosquitto, PostgreSQL) per i programmi che richiedevano file di chiavi non crittati e non in keystore, sono stati limitati gli accessi ai soli possessori delle chiavi e in sola lettura, e sono stati configurati appositamente i permessi anche nelle relative cartelle che li contengono. Le password per accedere ai keystore sono immesse da tastiera all'avvio del web server, è compito del responsabile software salvarle su un mezzo diverso. Le connessioni SSL generano chiavi simmetriche di sessione ogni volta. Le password per i keystore e truststore nel caso del webserver sono contenute dentro il codice, che pertanto deve essere cifrato per evitare reverse engineering. Non sono state messe password nei file di configurazione di hibernate dato che quando viene impacchettato nel jar sono in chiaro, bensì la password viene inserita nel codice java, è richiesta pertanto una tencica di obscuring per evitare la decompilazione. Il file che contiene username e password per Mosquitto è in chiaro ma salva password hashate, i permessi sono ristretti al solo possessore del file.</t>
-  </si>
-  <si>
     <t>Le password non sono salvate in chiaro ma con hash PBKDF2 da keycloak. Il database MariaDB è cifrato con algoritmo AES_CBC. I truststore sono cifrati e keystore anche. Per avviare il web server viene fatto uso di PBE con PBEWithMD5AndTripleDES sul file XML di configurazione. Le comunicazioni sono cifrate con algoritmi e chiave negoziate tramite crittografia asimmetrica RSA (2048 o 4096 bit). La mutua autenticazione avviene tramite certificati e firme digitali di una CA root self-signed. Il segreto condiviso per il client keycloak è embedded nel codice in versione cifrata, viene sbloccato dalla password che serve anche a sbloccare il keystore.</t>
   </si>
   <si>
     <t>Nel docugmento sono presenti le policy di cifratura  dei canali di comunicazione e del sistema.</t>
+  </si>
+  <si>
+    <t>Non c'è un DNS</t>
+  </si>
+  <si>
+    <t>Le chiavi RSA sono state generate tramite OpenSSL, distribuite fisicamente tra le varie componenti dell'infrastruttura (mount di volumi e segreti di docker), ove possibile (Spring, Keycloak) sono state messe in keystore protetti da password con entry a loro volte protette da password. Ove non possibile, (MariaDB, Mosquitto, PostgreSQL) per i programmi che richiedevano file di chiavi non crittati e non in keystore, sono stati limitati gli accessi ai soli possessori delle chiavi e in sola lettura, e sono stati configurati appositamente i permessi anche nelle relative cartelle che li contengono. Le password per accedere ai keystore del webserver sono immesse da tastiera all'avvio del web server, è compito del responsabile software salvarle su un mezzo diverso. Le connessioni SSL generano chiavi simmetriche di sessione ogni volta. Non sono state messe password nei file di configurazione di hibernate dato che quando viene impacchettato nel jar sono in chiaro, bensì la password viene inserita da tastiera all'avvio. Il file che contiene username e password per Mosquitto è in chiaro ma salva password hashate, i permessi sono ristretti al solo possessore del file.</t>
   </si>
 </sst>
 </file>
@@ -5601,8 +5601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752914C7-115F-4905-A8A7-15F56CC9E2E7}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G139" sqref="G139"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5658,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -5681,7 +5681,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -5704,7 +5704,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -5725,7 +5725,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5746,7 +5746,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -5761,13 +5761,13 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="18" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5813,7 +5813,7 @@
         <v>19</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5832,7 +5832,7 @@
         <v>381</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5853,7 +5853,7 @@
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5874,7 +5874,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5920,7 +5920,7 @@
         <v>383</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5989,7 +5989,7 @@
         <v>385</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6914,7 +6914,7 @@
         <v>144</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6928,16 +6928,16 @@
         <v>2</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>479</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>480</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>415</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6958,7 +6958,7 @@
         <v>148</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6981,7 +6981,7 @@
         <v>150</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6995,7 +6995,7 @@
         <v>2</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>416</v>
@@ -7004,7 +7004,7 @@
         <v>416</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7050,7 +7050,7 @@
         <v>156</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -8384,7 +8384,7 @@
         <v>308</v>
       </c>
       <c r="G139" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8405,7 +8405,7 @@
         <v>310</v>
       </c>
       <c r="G140" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8424,7 +8424,7 @@
         <v>436</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8445,7 +8445,7 @@
         <v>312</v>
       </c>
       <c r="G142" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8468,7 +8468,7 @@
         <v>314</v>
       </c>
       <c r="G143" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -8533,7 +8533,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>323</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>325</v>
       </c>
       <c r="G147" s="15" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -8576,7 +8576,7 @@
         <v>326</v>
       </c>
       <c r="G148" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8641,7 +8641,7 @@
         <v>332</v>
       </c>
       <c r="G151" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8685,7 +8685,7 @@
         <v>336</v>
       </c>
       <c r="G153" s="16" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -8708,7 +8708,7 @@
         <v>338</v>
       </c>
       <c r="G154" s="16" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -8731,7 +8731,7 @@
         <v>340</v>
       </c>
       <c r="G155" s="16" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -8768,7 +8768,7 @@
         <v>440</v>
       </c>
       <c r="G157" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -8789,7 +8789,7 @@
         <v>344</v>
       </c>
       <c r="G158" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -8812,7 +8812,7 @@
         <v>346</v>
       </c>
       <c r="G159" s="16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -8985,7 +8985,7 @@
         <v>367</v>
       </c>
       <c r="G168" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>